<commit_message>
Fix the example data
</commit_message>
<xml_diff>
--- a/decidim-dev/lib/decidim/dev/assets/dummy-dummies-example.xlsx
+++ b/decidim-dev/lib/decidim/dev/assets/dummy-dummies-example.xlsx
@@ -1,23 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierre/Code/PierreMesure/decidim/decidim-dev/lib/decidim/dev/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E352B9C-488F-A240-AA39-715EB31483E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+  <si>
+    <t>title/en</t>
+  </si>
+  <si>
+    <t>title/ca</t>
+  </si>
+  <si>
+    <t>title/es</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>translatable_text/en</t>
+  </si>
+  <si>
+    <t>translatable_text/ca</t>
+  </si>
+  <si>
+    <t>translatable_text/es</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Title text</t>
+  </si>
+  <si>
+    <t>Body text</t>
+  </si>
+  <si>
+    <t>Translatable text</t>
+  </si>
+  <si>
+    <t>Fake street 1</t>
+  </si>
+  <si>
+    <t>coordinates/latitude</t>
+  </si>
+  <si>
+    <t>coordinates/longitude</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Verdana"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Verdana"/>
-      <sz val="8"/>
     </font>
   </fonts>
   <fills count="2">
@@ -29,17 +83,33 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -199,7 +269,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="false"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -228,7 +298,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="false">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -237,7 +307,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -246,7 +316,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="false">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -362,73 +432,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" customFormat="false">
-      <c r="A1" s="0" t="str">
-        <v>title/en</v>
-      </c>
-      <c r="B1" s="0" t="str">
-        <v>title/ca</v>
-      </c>
-      <c r="C1" s="0" t="str">
-        <v>title/es</v>
-      </c>
-      <c r="D1" s="0" t="str">
-        <v>body</v>
-      </c>
-      <c r="E1" s="0" t="str">
-        <v>translatable_text/en</v>
-      </c>
-      <c r="F1" s="0" t="str">
-        <v>translatable_text/ca</v>
-      </c>
-      <c r="G1" s="0" t="str">
-        <v>translatable_text/es</v>
-      </c>
-      <c r="H1" s="0" t="str">
-        <v>address</v>
-      </c>
-      <c r="I1" s="0" t="str">
-        <v>latitude</v>
-      </c>
-      <c r="J1" s="0" t="str">
-        <v>longitude</v>
+    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" customFormat="false">
-      <c r="A2" s="0" t="str">
-        <v>Title text</v>
-      </c>
-      <c r="B2" s="0" t="str">
-        <v>Title text</v>
-      </c>
-      <c r="C2" s="0" t="str">
-        <v>Title text</v>
-      </c>
-      <c r="D2" s="0" t="str">
-        <v>Body text</v>
-      </c>
-      <c r="E2" s="0" t="str">
-        <v>Translatable text</v>
-      </c>
-      <c r="F2" s="0" t="str">
-        <v>Translatable text</v>
-      </c>
-      <c r="G2" s="0" t="str">
-        <v>Translatable text</v>
-      </c>
-      <c r="H2" s="0" t="str">
-        <v>Fake street 1</v>
-      </c>
-      <c r="I2" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="J2" s="0">
-        <v>1.0</v>
+    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>